<commit_message>
Adicionei horas e meta da prova
</commit_message>
<xml_diff>
--- a/estudo.xlsx
+++ b/estudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2023\Planilha Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E23A77-2EE3-482E-8B64-B650E1A3AB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029D5C1A-F29A-4930-A4FC-803725D6DF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{68954092-AD1A-404D-999D-5CAC431AE56B}"/>
   </bookViews>
@@ -69,7 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,11 +109,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,13 +264,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,12 +274,143 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -348,13 +470,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -370,118 +485,11 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -593,14 +601,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst/>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -613,9 +620,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -632,31 +638,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="84000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="1"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="20000"/>
-                </a:prstClr>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -672,9 +670,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -684,7 +685,6 @@
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -697,13 +697,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -713,45 +714,60 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$H$13:$H$19</c:f>
+              <c:f>Planilha1!$H$13:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>45024</c:v>
+                  <c:v>45027</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45025</c:v>
+                  <c:v>45028</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45026</c:v>
+                  <c:v>45029</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45027</c:v>
+                  <c:v>45030</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45028</c:v>
+                  <c:v>45031</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45029</c:v>
+                  <c:v>45032</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45030</c:v>
+                  <c:v>45033</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45034</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45035</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45036</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45038</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$G$13:$G$19</c:f>
+              <c:f>Planilha1!$G$13:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -762,15 +778,10 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-606B-4D16-BC2E-1974C5D065DB}"/>
@@ -778,7 +789,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -786,10 +796,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="41"/>
+        <c:smooth val="0"/>
         <c:axId val="541451512"/>
         <c:axId val="541451840"/>
-      </c:barChart>
+      </c:lineChart>
       <c:dateAx>
         <c:axId val="541451512"/>
         <c:scaling>
@@ -803,8 +813,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -815,12 +831,11 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst/>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -840,12 +855,39 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="541451512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1039,7 +1081,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1300,61 +1342,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="204">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200">
-      <a:effectLst/>
-    </cs:defRPr>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="68000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="85000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="1"/>
-        <a:tileRect/>
-      </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1362,163 +1376,127 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr/>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="84000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="1"/>
-      </a:gradFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="84000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="1"/>
-      </a:gradFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="84000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="1"/>
-        </a:gradFill>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="phClr"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="phClr">
-              <a:lumMod val="84000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="1"/>
-      </a:gradFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
   <cs:dataPointMarkerLayout symbol="circle" size="6"/>
@@ -1526,10 +1504,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1545,19 +1523,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1572,15 +1552,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="35000"/>
-          <a:lumOff val="65000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1591,14 +1571,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1610,14 +1590,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1629,7 +1609,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -1637,12 +1617,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1656,16 +1636,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1674,14 +1655,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1693,16 +1674,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1711,7 +1693,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1723,7 +1705,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -1731,7 +1713,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1739,15 +1721,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1762,14 +1744,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1781,14 +1763,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr kern="1200">
-      <a:effectLst/>
-    </cs:defRPr>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1797,14 +1777,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1813,7 +1792,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1829,13 +1808,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1848,7 +1825,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1860,7 +1837,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -2405,22 +2382,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1133475</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
         <xdr:cNvPr id="5" name="Agrupar 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D0E68B-FE13-50B8-288F-F5C619050D01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2428,9 +2405,9 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="762000" y="142875"/>
+          <a:off x="1323975" y="1238250"/>
           <a:ext cx="1714500" cy="723899"/>
-          <a:chOff x="276225" y="180975"/>
+          <a:chOff x="-1698096" y="-604087"/>
           <a:chExt cx="1733550" cy="685800"/>
         </a:xfrm>
       </xdr:grpSpPr>
@@ -2439,7 +2416,7 @@
           <xdr:cNvPr id="3" name="Retângulo: Cantos Arredondados 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E32F4F1-6C30-2BF1-1371-A5B209F8B14F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2447,7 +2424,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="276225" y="180975"/>
+            <a:off x="-1698096" y="-604087"/>
             <a:ext cx="1733550" cy="685800"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -2494,12 +2471,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$F$20">
+      <xdr:sp macro="" textlink="$F$25">
         <xdr:nvSpPr>
           <xdr:cNvPr id="4" name="CaixaDeTexto 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2642E5-6191-94E7-4831-FA3B72536BD9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2507,8 +2484,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="762000" y="514349"/>
-            <a:ext cx="657225" cy="257175"/>
+            <a:off x="-1125643" y="-297783"/>
+            <a:ext cx="814387" cy="257175"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2543,7 +2520,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:fld id="{44AFC0FC-6FD3-4F50-80F7-66267841D368}" type="TxLink">
+            <a:fld id="{8E4C6250-B49A-43D9-819F-84600EB6974B}" type="TxLink">
               <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
@@ -2551,8 +2528,7 @@
                 <a:latin typeface="Calibri"/>
                 <a:cs typeface="Calibri"/>
               </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>260</a:t>
+              <a:t>00:04:00</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
@@ -2564,22 +2540,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>447676</xdr:colOff>
+      <xdr:colOff>409576</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>176214</xdr:rowOff>
+      <xdr:rowOff>128589</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7176898-98D8-CE4F-FC47-241AC5E23286}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2615,7 +2591,7 @@
         <xdr:cNvPr id="9" name="Agrupar 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA6C1604-E7C7-D333-8C9F-3F36C27FB8F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2634,7 +2610,7 @@
           <xdr:cNvPr id="7" name="Gráfico 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07487B5-152D-7083-7926-56021661D38A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2655,7 +2631,7 @@
           <xdr:cNvPr id="8" name="CaixaDeTexto 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D590080-088D-2464-1CAD-A4C1FD670D47}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2701,7 +2677,7 @@
                 <a:cs typeface="Calibri"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>90%</a:t>
+              <a:t>73%</a:t>
             </a:fld>
             <a:endParaRPr lang="pt-BR" sz="1600" b="1">
               <a:solidFill>
@@ -2719,9 +2695,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>247651</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>19049</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -2804,7 +2780,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E682B998-35EF-8F2E-CFC7-A3AE75E04922}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2871,7 +2847,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE9C059-28D1-19C7-8D90-025609A5610B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2938,7 +2914,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40A64181-92BF-D89C-F184-A59E396E75CF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3005,7 +2981,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF849E0F-F595-C4FD-9208-3D504710B762}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3072,7 +3048,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C6888C-556B-C618-2DCB-48EC20564289}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3139,7 +3115,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3D4C3E-1EBE-BE8C-CC0E-9198174DEE87}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3206,7 +3182,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74992285-3ECA-A09B-3CBE-35E071D845AC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3250,18 +3226,96 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo: Cantos Arredondados 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56A96E9C-15E8-921E-8199-0E7DEA4F0A78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000125" y="114300"/>
+          <a:ext cx="2371725" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1" baseline="0"/>
+            <a:t>Data da Prova: 28/04  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1400" b="1" i="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" i="1" baseline="0"/>
+            <a:t>   Meta de nota: 8</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1200" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FA00E125-D57C-4032-9803-4D676D87ECDE}" name="Tabela4" displayName="Tabela4" ref="F2:H3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FA00E125-D57C-4032-9803-4D676D87ECDE}" name="Tabela4" displayName="Tabela4" ref="F2:H3" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="F2:H3" xr:uid="{FA00E125-D57C-4032-9803-4D676D87ECDE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6D55BD48-B700-493A-88E6-52624F52EB6B}" name="Total Questões Feitas" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{6D55BD48-B700-493A-88E6-52624F52EB6B}" name="Total Questões Feitas" dataDxfId="17">
       <calculatedColumnFormula>#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6E5F6484-9DED-4CD4-855B-9AC8909E293E}" name="Total Questões " dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{6499E56C-22A7-475A-A363-6265787BE1ED}" name="Progresso" dataDxfId="14" dataCellStyle="Porcentagem">
+    <tableColumn id="2" xr3:uid="{6E5F6484-9DED-4CD4-855B-9AC8909E293E}" name="Total Questões " dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{6499E56C-22A7-475A-A363-6265787BE1ED}" name="Progresso" dataDxfId="15" dataCellStyle="Porcentagem">
       <calculatedColumnFormula>Tabela4[[#This Row],[Total Questões Feitas]]/Tabela4[[#This Row],[Total Questões ]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3270,26 +3324,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDF3CD10-732E-4452-B203-6279E82B3EAE}" name="Tabela1" displayName="Tabela1" ref="F12:H20" totalsRowCount="1" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="F12:H19" xr:uid="{EDF3CD10-732E-4452-B203-6279E82B3EAE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDF3CD10-732E-4452-B203-6279E82B3EAE}" name="Tabela1" displayName="Tabela1" ref="F12:H25" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="F12:H24" xr:uid="{EDF3CD10-732E-4452-B203-6279E82B3EAE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F02F0E6F-BCDA-47A6-90F8-B9D7A1F9FDE5}" name="Tempo de Estudo" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{F02F0E6F-BCDA-47A6-90F8-B9D7A1F9FDE5}" name="Tempo de Estudo" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Tabela1[Tempo de Estudo])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{89A6553D-6C2B-4C7D-8441-A0F572740743}" name="Questões Feitas" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1AE10E38-43ED-4D74-B9F5-923F62ADAAE0}" name="Data" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{89A6553D-6C2B-4C7D-8441-A0F572740743}" name="Questões Feitas" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1AE10E38-43ED-4D74-B9F5-923F62ADAAE0}" name="Data" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8038EA5C-AE16-40D9-B83F-0D69241814C8}" name="Tabela2" displayName="Tabela2" ref="B12:D20" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8038EA5C-AE16-40D9-B83F-0D69241814C8}" name="Tabela2" displayName="Tabela2" ref="B12:D20" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B12:D20" xr:uid="{8038EA5C-AE16-40D9-B83F-0D69241814C8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D9FF6032-B424-47A8-8822-9B49ADB742F7}" name="Status" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A4032E4D-55E3-42EA-B1F0-5B0F71D77E0C}" name="Assuntos" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{A00C3982-4A55-46EF-ACE5-06A43302090A}" name="Comentários" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D9FF6032-B424-47A8-8822-9B49ADB742F7}" name="Status" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{A4032E4D-55E3-42EA-B1F0-5B0F71D77E0C}" name="Assuntos" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{A00C3982-4A55-46EF-ACE5-06A43302090A}" name="Comentários" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3592,10 +3646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A46FA4EC-9D98-4A3E-B26B-B7E7C8B0B8FB}">
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,14 +3678,14 @@
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F3" s="1">
         <f>Tabela1[[#Totals],[Questões Feitas]]</f>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1">
         <v>30</v>
       </c>
       <c r="H3" s="5">
         <f>Tabela4[[#This Row],[Total Questões Feitas]]/Tabela4[[#This Row],[Total Questões ]]</f>
-        <v>0.9</v>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3667,13 +3721,13 @@
       <c r="E11"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -3691,114 +3745,141 @@
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="F13" s="2">
-        <v>40</v>
+      <c r="D13" s="9"/>
+      <c r="F13" s="15">
+        <v>19.000462962962963</v>
       </c>
       <c r="G13" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H13" s="3">
-        <v>45024</v>
+        <v>45027</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="12"/>
-      <c r="F14" s="2">
-        <v>40</v>
+      <c r="D14" s="9"/>
+      <c r="F14" s="15">
+        <v>19.000578703703702</v>
       </c>
       <c r="G14" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H14" s="3">
-        <v>45025</v>
+        <v>45028</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="12"/>
-      <c r="F15" s="2">
-        <v>20</v>
+      <c r="D15" s="9"/>
+      <c r="F15" s="15">
+        <v>19.000578703703702</v>
       </c>
       <c r="G15" s="2">
         <v>3</v>
       </c>
       <c r="H15" s="3">
-        <v>45026</v>
+        <v>45029</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="12"/>
-      <c r="F16" s="2">
-        <v>40</v>
+      <c r="D16" s="9"/>
+      <c r="F16" s="15">
+        <v>19.000578703703702</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
       <c r="H16" s="3">
-        <v>45027</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="2">
-        <v>40</v>
+      <c r="D17" s="9"/>
+      <c r="F17" s="15">
+        <v>19.000578703703702</v>
       </c>
       <c r="G17" s="2">
         <v>3</v>
       </c>
       <c r="H17" s="3">
-        <v>45028</v>
+        <v>45031</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="12"/>
-      <c r="F18" s="2">
-        <v>40</v>
-      </c>
-      <c r="G18" s="2">
-        <v>3</v>
-      </c>
+      <c r="D18" s="9"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="3">
-        <v>45029</v>
+        <v>45032</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="12"/>
-      <c r="F19" s="2">
-        <v>40</v>
-      </c>
-      <c r="G19" s="2">
-        <v>3</v>
-      </c>
+      <c r="D19" s="9"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="3">
-        <v>45030</v>
+        <v>45033</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="F20" s="2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3">
+        <v>45034</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="15"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="3">
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="15"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="3">
+        <v>45036</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="15"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="3">
+        <v>45037</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="15"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="3">
+        <v>45038</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="15">
         <f>SUM(Tabela1[Tempo de Estudo])</f>
-        <v>260</v>
+        <v>95.002777777777766</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G25" s="2">
         <f>SUBTOTAL(109,Tabela1[Questões Feitas])</f>
-        <v>27</v>
+        <v>22</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>